<commit_message>
Auto stash before rebase of "dev"
</commit_message>
<xml_diff>
--- a/preprocessed_lemmatization.xlsx
+++ b/preprocessed_lemmatization.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>frustrar</t>
+          <t>frustração</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>satisfação pelar reconhecimento auto cobrança parir corresponder expectativa cansaço somatizações</t>
+          <t>satisfação pelar reconhecimento autocobrança parir corresponder expectativa cansaço somatizações</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>satisfação pelar reconhecimento auto cobrança parir corresponder expectativa cansaço somatizações</t>
+          <t>satisfação pelar reconhecimento autocobrança parir corresponder expectativa cansaço somatizações</t>
         </is>
       </c>
     </row>
@@ -753,14 +753,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>satisfação pelar reconhecimento auto cobrança parir corresponder expectativa cansaço somatizações</t>
+          <t>satisfação pelar reconhecimento autocobrança parir corresponder expectativa cansaço somatizações</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>colega telefonar pedir ajudar horar visitar famfamiliares trabalhar faculdade parir</t>
+          <t>colega telefonar pedir ajudar horar visitar familiar trabalhar faculdade parir</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -787,7 +787,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>colega telefonar pedir ajudar horar visitar famfamiliares trabalhar faculdade parir</t>
+          <t>colega telefonar pedir ajudar horar visitar familiar trabalhar faculdade parir</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>restrição alimentar casar sozsozinho disponibilidade comido discussão colega classe</t>
+          <t>restrição alimentar casar disponibilidade comido discussão colega classe</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -895,7 +895,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>restrição alimentar casar sozsozinho disponibilidade comido discussão colega classe</t>
+          <t>restrição alimentar casar disponibilidade comido discussão colega classe</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -922,7 +922,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>restrição alimentar casar sozsozinho disponibilidade comido discussão colega classe</t>
+          <t>restrição alimentar casar disponibilidade comido discussão colega classe</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -949,7 +949,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>restrição alimentar casar sozsozinho disponibilidade comido discussão colega classe</t>
+          <t>restrição alimentar casar disponibilidade comido discussão colega classe</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>controlo controlo aversivo pai</t>
+          <t>contracontrole controlo aversivo pai</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>privação comido horar comer casar aauto regrar comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
+          <t>privação comido horar comer casar autorregra comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1111,7 +1111,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>privação comido horar comer casar aauto regrar comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
+          <t>privação comido horar comer casar autorregra comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1138,7 +1138,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>privação comido horar comer casar aauto regrar comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
+          <t>privação comido horar comer casar autorregra comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1165,7 +1165,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>privação comido horar comer casar aauto regrar comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
+          <t>privação comido horar comer casar autorregra comer calórico comer quantidade parir conseguir vomitar facilidade discussão pai</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>auto confiança parir investir relacionamento amoroso</t>
+          <t>autoconfiança parir investir relacionamento amoroso</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>auto confiança parir investir relacionamento amoroso</t>
+          <t>autoconfiança parir investir relacionamento amoroso</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>auto confiança parir investir relacionamento amoroso</t>
+          <t>autoconfiança parir investir relacionamento amoroso</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>induzir vômito laxlaxantes usarurétdiuréticos restringirntosalimentos fazeros físico</t>
+          <t>induzir vômito laxante diurético restringir alimento exercício físico</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>auto confiança parir investir relacionamento amoroso</t>
+          <t>autoconfiança parir investir relacionamento amoroso</t>
         </is>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>controlo controlo aversivo pai</t>
+          <t>contracontrole controlo aversivo pai</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2029,7 +2029,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>discussão delegacia comum pai umar vítima estuprar atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoamoroso atima pego revólver parir suar cabeça</t>
+          <t>discussão delegacia comum pai umar vítima estrupo atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoroso vítima pego revólver parir suar cabeça</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>discussão delegacia comum pai umar vítima estuprar atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoamoroso atima pego revólver parir suar cabeça</t>
+          <t>discussão delegacia comum pai umar vítima estrupo atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoroso vítima pego revólver parir suar cabeça</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>verônica presença suicídio umar mulher trabalhar</t>
+          <t>verônica presenciar suicídio umar mulher trabalhar</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2083,7 +2083,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>discussão delegacia comum pai umar vítima estuprar atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoamoroso atima pego revólver parir suar cabeça</t>
+          <t>discussão delegacia comum pai umar vítima estrupo atirar acusar durante discussão revolver cair umar vítima golpe site relacionamento afetivo amoroso vítima pego revólver parir suar cabeça</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>verônica conseguir salvar mulher</t>
+          <t>verônica conseguir salvo mulher</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2353,7 +2353,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>verônica descobrir corrupção policiar regrar polpoliciaism ajudar pessoa</t>
+          <t>verônica descobrir corrupção policiar regrar policiar ajudar pessoa</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2380,7 +2380,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>verônica descobrir corrupção policiar regrar polpoliciaism ajudar pessoa</t>
+          <t>verônica descobrir corrupção policiar regrar policiar ajudar pessoa</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2542,12 +2542,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>interações social convite parir situação socsociais demandasr tomar decisõdecisões problemasem resolvidoresolvidos novasdades trabalhar</t>
+          <t>interações social convite parir situação social demandar tomar decisão problema resolvido oportunidade trabalhar</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>respostar passivo tímido p ex falir pensar dia decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
+          <t>respostar passivo tímido p ex falir pensar adir decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2569,12 +2569,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>interações social convite parir situação socsociais demandasr tomar decisõdecisões problemasem resolvidoresolvidos novasdades trabalhar</t>
+          <t>interações social convite parir situação social demandar tomar decisão problema resolvido oportunidade trabalhar</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>respostar passivo tímido p ex falir pensar dia decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
+          <t>respostar passivo tímido p ex falir pensar adir decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2596,12 +2596,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>interações social convite parir situação socsociais demandasr tomar decisõdecisões problemasem resolvidoresolvidos novasdades trabalhar</t>
+          <t>interações social convite parir situação social demandar tomar decisão problema resolvido oportunidade trabalhar</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>respostar passivo tímido p ex falir pensar dia decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
+          <t>respostar passivo tímido p ex falir pensar adir decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2623,12 +2623,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>interações social convite parir situação socsociais demandasr tomar decisõdecisões problemasem resolvidoresolvidos novasdades trabalhar</t>
+          <t>interações social convite parir situação social demandar tomar decisão problema resolvido oportunidade trabalhar</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>respostar passivo tímido p ex falir pensar dia decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
+          <t>respostar passivo tímido p ex falir pensar adir decisão medo julgar suar decisão encerrar assunto respondente medo ansiedade</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso tratrabalho desmarcarividades lazer</t>
+          <t>assumir responsabilidade pelar resolução relacionar filho desmarcar compromisso trabalhar desmarcar atividades lazer</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>sobrecarga pessoa aproveitar</t>
+          <t>sobrecarga pessoa aproveitar dela</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3109,12 +3109,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>convite namorar parir viajar convite amigo colega trabalhar parir saisair proposto trabaltrabalho problemasúde saudar demandass cuidar filho</t>
+          <t>convite namorar parir viajar convite amigo colega trabalhar parir sair proposto trabalhar problema saudar demandar relativo cuidar filho</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>aceitar convite parir sair atividades diferente aceitar proposto tratrabalho pediruda cuidar filho dividir responresponsabilidades cuidarúde alimentar ibem irs adequar adequar praticarfísicas</t>
+          <t>aceitar convite parir sair atividades diferente aceitar proposto trabalhar pedir ajudar cuidar filho dividir responsabilidade cuidar saudar alimentar médico adequar praticar atividades físico</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3136,12 +3136,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>convite namorar parir viajar convite amigo colega trabalhar parir saisair proposto trabaltrabalho problemasúde saudar demandass cuidar filho</t>
+          <t>convite namorar parir viajar convite amigo colega trabalhar parir sair proposto trabalhar problema saudar demandar relativo cuidar filho</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>aceitar convite parir sair atividades diferente aceitar proposto tratrabalho pediruda cuidar filho dividir responresponsabilidades cuidarúde alimentar ibem irs adequar adequar praticarfísicas</t>
+          <t>aceitar convite parir sair atividades diferente aceitar proposto trabalhar pedir ajudar cuidar filho dividir responsabilidade cuidar saudar alimentar médico adequar praticar atividades físico</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3163,12 +3163,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>convite namorar parir viajar convite amigo colega trabalhar parir saisair proposto trabaltrabalho problemasúde saudar demandass cuidar filho</t>
+          <t>convite namorar parir viajar convite amigo colega trabalhar parir sair proposto trabalhar problema saudar demandar relativo cuidar filho</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>aceitar convite parir sair atividades diferente aceitar proposto tratrabalho pediruda cuidar filho dividir responresponsabilidades cuidarúde alimentar ibem irs adequar adequar praticarfísicas</t>
+          <t>aceitar convite parir sair atividades diferente aceitar proposto trabalhar pedir ajudar cuidar filho dividir responsabilidade cuidar saudar alimentar médico adequar praticar atividades físico</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3190,12 +3190,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>convite namorar parir viajar convite amigo colega trabalhar parir saisair proposto trabaltrabalho problemasúde saudar demandass cuidar filho</t>
+          <t>convite namorar parir viajar convite amigo colega trabalhar parir sair proposto trabalhar problema saudar demandar relativo cuidar filho</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>aceitar convite parir sair atividades diferente aceitar proposto tratrabalho pediruda cuidar filho dividir responresponsabilidades cuidarúde alimentar ibem irs adequar adequar praticarfísicas</t>
+          <t>aceitar convite parir sair atividades diferente aceitar proposto trabalhar pedir ajudar cuidar filho dividir responsabilidade cuidar saudar alimentar médico adequar praticar atividades físico</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3330,7 +3330,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>assertividade argumentar expressar opinião sensentimentos recusardidos formar direta</t>
+          <t>assertividade argumentar expressar opinião sentimento recusar pedir formar direta</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3411,12 +3411,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>riscar pessoa receber pedir</t>
+          <t>riscar pessoa recusar pedir</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3438,7 +3438,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3542,7 +3542,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>buscar solução solicitar ajuajuda fazerdidos diretos envolver oportunidade trabaltrabalho tomarões decisão expressartos necessidade maneiro claro</t>
+          <t>buscar solução solicitar ajudar pedir diretos envolver oportunidade trabalhar tomar decisão expressar sentimento necessidade maneiro claro</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>hiperplasia</t>
+          <t>hiperlalia</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3700,7 +3700,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>hiperplasia</t>
+          <t>hiperlalia</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3857,7 +3857,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>regrar regrar pai sobrar matar pessoa família unir brigar auto regrar umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
+          <t>regrar regrar pai sobrar matar pessoa família unir brigar autorregras umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>regrar regrar pai sobrar matar pessoa família unir brigar auto regrar umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
+          <t>regrar regrar pai sobrar matar pessoa família unir brigar autorregras umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3911,7 +3911,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>regrar regrar pai sobrar matar pessoa família unir brigar auto regrar umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
+          <t>regrar regrar pai sobrar matar pessoa família unir brigar autorregras umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3934,7 +3934,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>regrar regrar pai sobrar matar pessoa família unir brigar auto regrar umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
+          <t>regrar regrar pai sobrar matar pessoa família unir brigar autorregras umar pessoa devir gostar mim sds solicitação ajudar amigo familiar</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>atividades normal aceitável pai evitar paipai fingee escutaescuta respostandente ansiedade</t>
+          <t>atividades normal aceitável pai evitar pai fingir escutar respostar respondente ansiedade</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>atividades normal aceitável pai evitar paipai fingee escutaescuta respostandente ansiedade</t>
+          <t>atividades normal aceitável pai evitar pai fingir escutar respostar respondente ansiedade</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>aumentar voz xingar discutir caro raivar conseguir pensarclaramente respostass respondente transpiração sensação estressado</t>
+          <t>aumentar voz xingar discutir caro raivar conseguir pensar claramente respostar respondente transpiração sensação estressado</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>aumentar voz xingar discutir caro raivar conseguir pensarclaramente respostass respondente transpiração sensação estressado</t>
+          <t>aumentar voz xingar discutir caro raivar conseguir pensar claramente respostar respondente transpiração sensação estressado</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4660,7 +4660,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>aumentar voz xingar discutir caro raivar conseguir pensarclaramente respostass respondente transpiração sensação estressado</t>
+          <t>aumentar voz xingar discutir caro raivar conseguir pensar claramente respostar respondente transpiração sensação estressado</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5331,7 +5331,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>dia comportamento procrastinador véspera lembrar queaconteceu dizz esquecer</t>
+          <t>adir comportamento procrastinador véspera lembrar acontecer esquecer</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5358,7 +5358,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>dia comportamento procrastinador véspera lembrar queaconteceu dizz esquecer</t>
+          <t>adir comportamento procrastinador véspera lembrar acontecer esquecer</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">

</xml_diff>